<commit_message>
Hardware revision v0.3.0 (#16)
* Split backlight into two zones, removed status LEDs, reduced y size by 1mm

* Made firmware compatible with v0.3.0 (doesn't make use of dual backlight controls yet), refactoring

* Improved Case Generator script, added presets for Fairphone 4 and Samsung Galaxy A54

* Finalisation of v0.3.0 PCB

* License/Version header for firmware

* Removed generated stl
</commit_message>
<xml_diff>
--- a/KiCad/FairberryMainboard/cpl/BOM.xlsx
+++ b/KiCad/FairberryMainboard/cpl/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">25V 1uF X5R ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2</t>
+    <t xml:space="preserve">C1</t>
   </si>
   <si>
     <t xml:space="preserve">C52923</t>
@@ -142,52 +142,22 @@
     <t xml:space="preserve">16V 100nF X7R ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t xml:space="preserve">C3</t>
+    <t xml:space="preserve">C2,C3</t>
   </si>
   <si>
     <t xml:space="preserve">C1525</t>
   </si>
   <si>
-    <t xml:space="preserve">±1% 1/16W Thick Film Resistors 50V ±100ppm/℃ -55℃~+155℃ 470Ω 0402 Chip Resistor - Surface Mount ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25117 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">±1% 1/16W Thick Film Resistors 50V ±100ppm/℃ -55℃~+155℃ 680Ω 0402 Chip Resistor - Surface Mount ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0402 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5mA 28.5mcd 3.1V 468nm Colorless transparence -40℃~+85℃ 465nm~475nm blue 120° 110mW 0603 Light Emitting Diodes (LED) ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED_0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C72041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20mA 180mcd 2.3V 591nm Colorless transparence -40℃~+85℃ 585.5nm~591.5nm yellow 120° 60mW 0603 Light Emitting Diodes (LED) ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C72038</t>
+    <t xml:space="preserve">0.4mm 2 24P Brick nogging Female SMD,P=0.4mm Mezzanine Connectors (Board to Board) ROHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD,P=0.4mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3640874</t>
   </si>
 </sst>
 </file>
@@ -306,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -343,16 +313,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -435,7 +401,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8828125" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -558,73 +524,43 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>31</v>
       </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="A11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Hardware revision v0.3.0 (#16) (#19)
* Split backlight into two zones, removed status LEDs, reduced y size by 1mm

* Made firmware compatible with v0.3.0 (doesn't make use of dual backlight controls yet), refactoring

* Improved Case Generator script, added presets for Fairphone 4 and Samsung Galaxy A54

* Finalisation of v0.3.0 PCB

* License/Version header for firmware

* Removed generated stl
</commit_message>
<xml_diff>
--- a/KiCad/FairberryMainboard/cpl/BOM.xlsx
+++ b/KiCad/FairberryMainboard/cpl/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">25V 1uF X5R ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2</t>
+    <t xml:space="preserve">C1</t>
   </si>
   <si>
     <t xml:space="preserve">C52923</t>
@@ -142,52 +142,22 @@
     <t xml:space="preserve">16V 100nF X7R ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t xml:space="preserve">C3</t>
+    <t xml:space="preserve">C2,C3</t>
   </si>
   <si>
     <t xml:space="preserve">C1525</t>
   </si>
   <si>
-    <t xml:space="preserve">±1% 1/16W Thick Film Resistors 50V ±100ppm/℃ -55℃~+155℃ 470Ω 0402 Chip Resistor - Surface Mount ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25117 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">±1% 1/16W Thick Film Resistors 50V ±100ppm/℃ -55℃~+155℃ 680Ω 0402 Chip Resistor - Surface Mount ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0402 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5mA 28.5mcd 3.1V 468nm Colorless transparence -40℃~+85℃ 465nm~475nm blue 120° 110mW 0603 Light Emitting Diodes (LED) ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED_0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C72041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20mA 180mcd 2.3V 591nm Colorless transparence -40℃~+85℃ 585.5nm~591.5nm yellow 120° 60mW 0603 Light Emitting Diodes (LED) ROHS Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C72038</t>
+    <t xml:space="preserve">0.4mm 2 24P Brick nogging Female SMD,P=0.4mm Mezzanine Connectors (Board to Board) ROHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD,P=0.4mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3640874</t>
   </si>
 </sst>
 </file>
@@ -306,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -343,16 +313,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -435,7 +401,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8828125" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -558,73 +524,43 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>31</v>
       </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="A11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>